<commit_message>
PRJ0018886_Hierarchy Viewer+ Time recordManager(PArtial changes)
</commit_message>
<xml_diff>
--- a/TestData/TMTI0003744_TimeRecordManager_VerifyTimeEntriesInTimeRecordManager_RoundOffToFirstDecimalPlaceOfAnHour.xlsx
+++ b/TestData/TMTI0003744_TimeRecordManager_VerifyTimeEntriesInTimeRecordManager_RoundOffToFirstDecimalPlaceOfAnHour.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hgandhi1012\source\repos\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vijay.kumar\source\repos\SalesForce_Project\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F609EE-7A85-4FC1-99C0-9488ECFC952D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12756" windowHeight="2976"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="5" r:id="rId1"/>
@@ -17,17 +18,28 @@
     <sheet name="SummaryLogs" sheetId="7" r:id="rId3"/>
     <sheet name="DetailLogs" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Global Search User</t>
   </si>
@@ -96,12 +108,21 @@
   </si>
   <si>
     <t>Yuka Itami</t>
+  </si>
+  <si>
+    <t>E - Akin_PIMCO-Akin Gump Strauss Hauer &amp; Feld LLP-FVA-102657</t>
+  </si>
+  <si>
+    <t>Type to filter projects...</t>
+  </si>
+  <si>
+    <t>Akin_PIMCO-Akin Gump Strauss Hauer &amp; Feld LLP-FVA-102657</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,11 +443,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,24 +473,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="57.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -488,10 +511,13 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -506,6 +532,15 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -516,21 +551,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -544,9 +579,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -556,6 +591,9 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -564,16 +602,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -593,8 +631,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>

</xml_diff>